<commit_message>
Create Resiliency file at the end of process
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smithm/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smithm/GitHub/ARI-for-Reliability-Review/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98AB7CD1-11B9-DE4C-B963-66495277FFA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CB7FFD1-A2E1-0248-94C4-AB01ECD10FE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3920" yWindow="500" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{94597F4E-FC60-4FA1-B7E2-C7C1A109AD66}"/>
+    <workbookView xWindow="3920" yWindow="760" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{94597F4E-FC60-4FA1-B7E2-C7C1A109AD66}"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
     <sheet name="Temp" sheetId="3" r:id="rId2"/>
     <sheet name="RTO &amp; RPO Assessment Template" sheetId="2" r:id="rId3"/>
-    <sheet name="Combine" sheetId="5" r:id="rId4"/>
+    <sheet name="Inventory" sheetId="5" r:id="rId4"/>
     <sheet name="App RTO &amp; RPO Assessment" sheetId="4" state="hidden" r:id="rId5"/>
   </sheets>
   <definedNames>
@@ -757,16 +757,16 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="7" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -778,17 +778,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1600,7 +1600,7 @@
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="E1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q31" sqref="Q31"/>
+      <selection pane="bottomLeft" activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1632,37 +1632,37 @@
       <c r="V1" s="1"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37" t="s">
+      <c r="C3" s="38"/>
+      <c r="D3" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37" t="s">
+      <c r="E3" s="38"/>
+      <c r="F3" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="37"/>
+      <c r="G3" s="38"/>
       <c r="I3" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="N3" s="37" t="s">
+      <c r="N3" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="O3" s="37"/>
-      <c r="P3" s="37" t="s">
+      <c r="O3" s="38"/>
+      <c r="P3" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="Q3" s="37"/>
-      <c r="R3" s="37" t="s">
+      <c r="Q3" s="38"/>
+      <c r="R3" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="S3" s="37"/>
-      <c r="T3" s="36" t="s">
+      <c r="S3" s="38"/>
+      <c r="T3" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="U3" s="36"/>
+      <c r="U3" s="37"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" s="21" t="s">
@@ -4173,26 +4173,26 @@
         <v>121</v>
       </c>
       <c r="G7" s="42"/>
-      <c r="H7" s="45" t="s">
+      <c r="H7" s="39" t="s">
         <v>122</v>
       </c>
-      <c r="I7" s="45"/>
-      <c r="J7" s="44" t="s">
+      <c r="I7" s="39"/>
+      <c r="J7" s="43" t="s">
         <v>121</v>
       </c>
-      <c r="K7" s="44"/>
-      <c r="L7" s="45" t="s">
+      <c r="K7" s="43"/>
+      <c r="L7" s="39" t="s">
         <v>122</v>
       </c>
-      <c r="M7" s="45"/>
-      <c r="N7" s="44" t="s">
+      <c r="M7" s="39"/>
+      <c r="N7" s="43" t="s">
         <v>121</v>
       </c>
-      <c r="O7" s="44"/>
-      <c r="P7" s="45" t="s">
+      <c r="O7" s="43"/>
+      <c r="P7" s="39" t="s">
         <v>122</v>
       </c>
-      <c r="Q7" s="45"/>
+      <c r="Q7" s="39"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
@@ -8813,56 +8813,56 @@
       <c r="O82" s="40"/>
       <c r="P82" s="40"/>
       <c r="Q82" s="40"/>
-      <c r="S82" s="39" t="s">
+      <c r="S82" s="46" t="s">
         <v>125</v>
       </c>
-      <c r="T82" s="39"/>
-      <c r="U82" s="39"/>
-      <c r="V82" s="39"/>
-      <c r="W82" s="39"/>
-      <c r="X82" s="39"/>
+      <c r="T82" s="46"/>
+      <c r="U82" s="46"/>
+      <c r="V82" s="46"/>
+      <c r="W82" s="46"/>
+      <c r="X82" s="46"/>
     </row>
     <row r="83" spans="1:24" x14ac:dyDescent="0.2">
       <c r="F83" s="41" t="s">
         <v>121</v>
       </c>
       <c r="G83" s="42"/>
-      <c r="H83" s="43" t="s">
+      <c r="H83" s="44" t="s">
         <v>122</v>
       </c>
-      <c r="I83" s="43"/>
-      <c r="J83" s="44" t="s">
+      <c r="I83" s="44"/>
+      <c r="J83" s="43" t="s">
         <v>121</v>
       </c>
-      <c r="K83" s="44"/>
-      <c r="L83" s="43" t="s">
+      <c r="K83" s="43"/>
+      <c r="L83" s="44" t="s">
         <v>122</v>
       </c>
-      <c r="M83" s="43"/>
-      <c r="N83" s="44" t="s">
+      <c r="M83" s="44"/>
+      <c r="N83" s="43" t="s">
         <v>121</v>
       </c>
-      <c r="O83" s="44"/>
-      <c r="P83" s="43" t="s">
+      <c r="O83" s="43"/>
+      <c r="P83" s="44" t="s">
         <v>122</v>
       </c>
-      <c r="Q83" s="43"/>
-      <c r="S83" s="38" t="s">
+      <c r="Q83" s="44"/>
+      <c r="S83" s="45" t="s">
         <v>126</v>
       </c>
-      <c r="T83" s="38" t="s">
+      <c r="T83" s="45" t="s">
         <v>127</v>
       </c>
-      <c r="U83" s="38" t="s">
+      <c r="U83" s="45" t="s">
         <v>128</v>
       </c>
-      <c r="V83" s="38" t="s">
+      <c r="V83" s="45" t="s">
         <v>129</v>
       </c>
-      <c r="W83" s="38" t="s">
+      <c r="W83" s="45" t="s">
         <v>130</v>
       </c>
-      <c r="X83" s="38" t="s">
+      <c r="X83" s="45" t="s">
         <v>131</v>
       </c>
     </row>
@@ -8918,12 +8918,12 @@
       <c r="Q84" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="S84" s="38"/>
-      <c r="T84" s="38"/>
-      <c r="U84" s="38"/>
-      <c r="V84" s="38"/>
-      <c r="W84" s="38"/>
-      <c r="X84" s="38"/>
+      <c r="S84" s="45"/>
+      <c r="T84" s="45"/>
+      <c r="U84" s="45"/>
+      <c r="V84" s="45"/>
+      <c r="W84" s="45"/>
+      <c r="X84" s="45"/>
     </row>
     <row r="85" spans="1:24" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A85" s="4" t="str">
@@ -15483,6 +15483,22 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="X83:X84"/>
+    <mergeCell ref="S82:X82"/>
+    <mergeCell ref="S83:S84"/>
+    <mergeCell ref="T83:T84"/>
+    <mergeCell ref="U83:U84"/>
+    <mergeCell ref="V83:V84"/>
+    <mergeCell ref="W83:W84"/>
+    <mergeCell ref="F82:I82"/>
+    <mergeCell ref="J82:M82"/>
+    <mergeCell ref="N82:Q82"/>
+    <mergeCell ref="F83:G83"/>
+    <mergeCell ref="H83:I83"/>
+    <mergeCell ref="J83:K83"/>
+    <mergeCell ref="L83:M83"/>
+    <mergeCell ref="N83:O83"/>
+    <mergeCell ref="P83:Q83"/>
     <mergeCell ref="P7:Q7"/>
     <mergeCell ref="N6:Q6"/>
     <mergeCell ref="F6:I6"/>
@@ -15492,22 +15508,6 @@
     <mergeCell ref="J7:K7"/>
     <mergeCell ref="L7:M7"/>
     <mergeCell ref="N7:O7"/>
-    <mergeCell ref="F82:I82"/>
-    <mergeCell ref="J82:M82"/>
-    <mergeCell ref="N82:Q82"/>
-    <mergeCell ref="F83:G83"/>
-    <mergeCell ref="H83:I83"/>
-    <mergeCell ref="J83:K83"/>
-    <mergeCell ref="L83:M83"/>
-    <mergeCell ref="N83:O83"/>
-    <mergeCell ref="P83:Q83"/>
-    <mergeCell ref="X83:X84"/>
-    <mergeCell ref="S82:X82"/>
-    <mergeCell ref="S83:S84"/>
-    <mergeCell ref="T83:T84"/>
-    <mergeCell ref="U83:U84"/>
-    <mergeCell ref="V83:V84"/>
-    <mergeCell ref="W83:W84"/>
   </mergeCells>
   <conditionalFormatting sqref="H79">
     <cfRule type="cellIs" dxfId="47" priority="24" operator="lessThanOrEqual">
@@ -15633,28 +15633,28 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="36" t="s">
         <v>148</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="36" t="s">
         <v>149</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="D1" s="36" t="s">
         <v>150</v>
       </c>
-      <c r="E1" s="46" t="s">
+      <c r="E1" s="36" t="s">
         <v>151</v>
       </c>
-      <c r="F1" s="46" t="s">
+      <c r="F1" s="36" t="s">
         <v>152</v>
       </c>
     </row>
@@ -15740,30 +15740,30 @@
       <c r="P6" s="40"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="E7" s="44" t="s">
+      <c r="E7" s="43" t="s">
         <v>121</v>
       </c>
-      <c r="F7" s="44"/>
-      <c r="G7" s="45" t="s">
+      <c r="F7" s="43"/>
+      <c r="G7" s="39" t="s">
         <v>122</v>
       </c>
-      <c r="H7" s="45"/>
-      <c r="I7" s="44" t="s">
+      <c r="H7" s="39"/>
+      <c r="I7" s="43" t="s">
         <v>121</v>
       </c>
-      <c r="J7" s="44"/>
-      <c r="K7" s="45" t="s">
+      <c r="J7" s="43"/>
+      <c r="K7" s="39" t="s">
         <v>122</v>
       </c>
-      <c r="L7" s="45"/>
-      <c r="M7" s="44" t="s">
+      <c r="L7" s="39"/>
+      <c r="M7" s="43" t="s">
         <v>121</v>
       </c>
-      <c r="N7" s="44"/>
-      <c r="O7" s="45" t="s">
+      <c r="N7" s="43"/>
+      <c r="O7" s="39" t="s">
         <v>122</v>
       </c>
-      <c r="P7" s="45"/>
+      <c r="P7" s="39"/>
     </row>
     <row r="8" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
@@ -19861,30 +19861,30 @@
       <c r="P82" s="40"/>
     </row>
     <row r="83" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="E83" s="44" t="s">
+      <c r="E83" s="43" t="s">
         <v>121</v>
       </c>
-      <c r="F83" s="44"/>
-      <c r="G83" s="43" t="s">
+      <c r="F83" s="43"/>
+      <c r="G83" s="44" t="s">
         <v>122</v>
       </c>
-      <c r="H83" s="43"/>
-      <c r="I83" s="44" t="s">
+      <c r="H83" s="44"/>
+      <c r="I83" s="43" t="s">
         <v>121</v>
       </c>
-      <c r="J83" s="44"/>
-      <c r="K83" s="43" t="s">
+      <c r="J83" s="43"/>
+      <c r="K83" s="44" t="s">
         <v>122</v>
       </c>
-      <c r="L83" s="43"/>
-      <c r="M83" s="44" t="s">
+      <c r="L83" s="44"/>
+      <c r="M83" s="43" t="s">
         <v>121</v>
       </c>
-      <c r="N83" s="44"/>
-      <c r="O83" s="43" t="s">
+      <c r="N83" s="43"/>
+      <c r="O83" s="44" t="s">
         <v>122</v>
       </c>
-      <c r="P83" s="43"/>
+      <c r="P83" s="44"/>
     </row>
     <row r="84" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
@@ -24547,6 +24547,15 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="E82:H82"/>
+    <mergeCell ref="I82:L82"/>
+    <mergeCell ref="M82:P82"/>
+    <mergeCell ref="E83:F83"/>
+    <mergeCell ref="G83:H83"/>
+    <mergeCell ref="I83:J83"/>
+    <mergeCell ref="K83:L83"/>
+    <mergeCell ref="M83:N83"/>
+    <mergeCell ref="O83:P83"/>
     <mergeCell ref="E6:H6"/>
     <mergeCell ref="I6:L6"/>
     <mergeCell ref="M6:P6"/>
@@ -24556,15 +24565,6 @@
     <mergeCell ref="K7:L7"/>
     <mergeCell ref="M7:N7"/>
     <mergeCell ref="O7:P7"/>
-    <mergeCell ref="E82:H82"/>
-    <mergeCell ref="I82:L82"/>
-    <mergeCell ref="M82:P82"/>
-    <mergeCell ref="E83:F83"/>
-    <mergeCell ref="G83:H83"/>
-    <mergeCell ref="I83:J83"/>
-    <mergeCell ref="K83:L83"/>
-    <mergeCell ref="M83:N83"/>
-    <mergeCell ref="O83:P83"/>
   </mergeCells>
   <conditionalFormatting sqref="G79">
     <cfRule type="cellIs" dxfId="23" priority="23" operator="lessThanOrEqual">
@@ -24695,6 +24695,26 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="80b0474e-37b4-4751-81bc-12d5121181de">
+      <UserInfo>
+        <DisplayName>Smith Mangmeetakun</DisplayName>
+        <AccountId>72</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="670f2bc3-833b-4a76-b13f-f7d6db0b8f4d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F523F0DE61C01647AADD57BC023588A4" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ee28fff2fb8673b821d9cefaa23fecad">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="670f2bc3-833b-4a76-b13f-f7d6db0b8f4d" xmlns:ns3="230e9df3-be65-4c73-a93b-d1236ebd677e" xmlns:ns4="80b0474e-37b4-4751-81bc-12d5121181de" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="89cbad1f211539c7601732b6d3a7f38a" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -24951,26 +24971,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="80b0474e-37b4-4751-81bc-12d5121181de">
-      <UserInfo>
-        <DisplayName>Smith Mangmeetakun</DisplayName>
-        <AccountId>72</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="670f2bc3-833b-4a76-b13f-f7d6db0b8f4d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73B3A99D-AAD3-4558-A49E-D0B79DE8CAD4}">
   <ds:schemaRefs>
@@ -24980,6 +24980,19 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{626FDD16-2397-4697-ACDD-4A4A15E67330}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="80b0474e-37b4-4751-81bc-12d5121181de"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="670f2bc3-833b-4a76-b13f-f7d6db0b8f4d"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EFD77F6C-2665-4616-8E0C-961858CD74CD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -25000,19 +25013,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{626FDD16-2397-4697-ACDD-4A4A15E67330}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="80b0474e-37b4-4751-81bc-12d5121181de"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="670f2bc3-833b-4a76-b13f-f7d6db0b8f4d"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Standard" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" contentBits="0" removed="0"/>

</xml_diff>